<commit_message>
added geospatial visualization and parallelization to robust pipeline design
</commit_message>
<xml_diff>
--- a/examples/Multi-regional Energy System Workflow/InputData/SpatialData/ElectricGrid/ACcableExistingCapacity_GW_el.xlsx
+++ b/examples/Multi-regional Energy System Workflow/InputData/SpatialData/ElectricGrid/ACcableExistingCapacity_GW_el.xlsx
@@ -1,15 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Models\FINE_GITLAB_TSA\FINE\examples\Multi-regional Energy System Workflow\InputData\SpatialData\ElectricGrid\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
@@ -43,8 +48,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -103,15 +108,23 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -153,7 +166,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -185,9 +198,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -219,6 +233,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -394,14 +409,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -427,7 +442,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:9">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -435,65 +450,65 @@
         <v>0</v>
       </c>
       <c r="C2">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="D2">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="E2">
-        <v>2.395772677029271</v>
+        <v>0</v>
       </c>
       <c r="F2">
-        <v>3.262664106217494</v>
+        <v>18</v>
       </c>
       <c r="G2">
-        <v>2.395772677029271</v>
+        <v>4</v>
       </c>
       <c r="H2">
         <v>0</v>
       </c>
       <c r="I2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B3">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="C3">
         <v>0</v>
       </c>
       <c r="D3">
-        <v>8.905339227115384</v>
+        <v>10</v>
       </c>
       <c r="E3">
-        <v>4.791545354058541</v>
+        <v>0</v>
       </c>
       <c r="F3">
         <v>0</v>
       </c>
       <c r="G3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="H3">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="I3">
-        <v>9.866800630396865</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B4">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="C4">
-        <v>8.905339227115384</v>
+        <v>10</v>
       </c>
       <c r="D4">
         <v>0</v>
@@ -502,7 +517,7 @@
         <v>0</v>
       </c>
       <c r="F4">
-        <v>8.731960941277739</v>
+        <v>0</v>
       </c>
       <c r="G4">
         <v>0</v>
@@ -511,18 +526,18 @@
         <v>0</v>
       </c>
       <c r="I4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B5">
-        <v>2.395772677029271</v>
+        <v>0</v>
       </c>
       <c r="C5">
-        <v>4.791545354058541</v>
+        <v>0</v>
       </c>
       <c r="D5">
         <v>0</v>
@@ -531,39 +546,39 @@
         <v>0</v>
       </c>
       <c r="F5">
-        <v>5.737245094991149</v>
+        <v>0</v>
       </c>
       <c r="G5">
-        <v>13.38165133419639</v>
+        <v>12</v>
       </c>
       <c r="H5">
-        <v>0.9456997409326068</v>
+        <v>2.4</v>
       </c>
       <c r="I5">
-        <v>3.593659015543908</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B6">
-        <v>3.262664106217494</v>
+        <v>18</v>
       </c>
       <c r="C6">
         <v>0</v>
       </c>
       <c r="D6">
-        <v>8.731960941277739</v>
+        <v>0</v>
       </c>
       <c r="E6">
-        <v>5.737245094991149</v>
+        <v>0</v>
       </c>
       <c r="F6">
         <v>0</v>
       </c>
       <c r="G6">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="H6">
         <v>0</v>
@@ -572,36 +587,36 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:9">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B7">
-        <v>2.395772677029271</v>
+        <v>4</v>
       </c>
       <c r="C7">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="D7">
         <v>0</v>
       </c>
       <c r="E7">
-        <v>13.38165133419639</v>
+        <v>12</v>
       </c>
       <c r="F7">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="G7">
         <v>0</v>
       </c>
       <c r="H7">
-        <v>1.796829507771953</v>
+        <v>0</v>
       </c>
       <c r="I7">
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:9">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>6</v>
       </c>
@@ -609,42 +624,42 @@
         <v>0</v>
       </c>
       <c r="C8">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="D8">
         <v>0</v>
       </c>
       <c r="E8">
-        <v>0.9456997409326068</v>
+        <v>2.4</v>
       </c>
       <c r="F8">
         <v>0</v>
       </c>
       <c r="G8">
-        <v>1.796829507771953</v>
+        <v>0</v>
       </c>
       <c r="H8">
         <v>0</v>
       </c>
       <c r="I8">
-        <v>6.178571640759698</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B9">
-        <v>0</v>
+        <v>2.5</v>
       </c>
       <c r="C9">
-        <v>9.866800630396865</v>
+        <v>0</v>
       </c>
       <c r="D9">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E9">
-        <v>3.593659015543908</v>
+        <v>0</v>
       </c>
       <c r="F9">
         <v>0</v>
@@ -653,7 +668,7 @@
         <v>0</v>
       </c>
       <c r="H9">
-        <v>6.178571640759698</v>
+        <v>0</v>
       </c>
       <c r="I9">
         <v>0</v>

</xml_diff>